<commit_message>
resloved conflicts in admin
</commit_message>
<xml_diff>
--- a/MainAssignmnet/MoviesInfo.xlsx
+++ b/MainAssignmnet/MoviesInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vuchander\Python_Track\MainAssignmnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444B7874-5B34-4DAC-957B-C5B3BC60EBB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E5D4E2-C47E-4978-8F6B-A0391DC15FA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Moviename</t>
   </si>
@@ -76,13 +76,10 @@
     <t>rajamouli</t>
   </si>
   <si>
-    <t>dammu</t>
-  </si>
-  <si>
-    <t>2hr45min</t>
-  </si>
-  <si>
-    <t>ntr</t>
+    <t>10:00-1:30</t>
+  </si>
+  <si>
+    <t>2 :00-5:30</t>
   </si>
   <si>
     <t>RRR</t>
@@ -92,18 +89,6 @@
   </si>
   <si>
     <t>Ramcharan,Ntr,aliaBhatt</t>
-  </si>
-  <si>
-    <t>2:00-5:00</t>
-  </si>
-  <si>
-    <t>10:00-1:30</t>
-  </si>
-  <si>
-    <t>10:00-1:00</t>
-  </si>
-  <si>
-    <t>2 :00-5:30</t>
   </si>
   <si>
     <t>2:00-5:30</t>
@@ -142,9 +127,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,10 +491,10 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -525,36 +509,36 @@
         <v>15</v>
       </c>
       <c r="M2">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
       </c>
       <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>10</v>
@@ -566,48 +550,7 @@
         <v>15</v>
       </c>
       <c r="M3">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>15</v>
-      </c>
-      <c r="L4">
-        <v>15</v>
-      </c>
-      <c r="M4">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checked all functionalities and solved issues
</commit_message>
<xml_diff>
--- a/MainAssignmnet/MoviesInfo.xlsx
+++ b/MainAssignmnet/MoviesInfo.xlsx
@@ -396,7 +396,7 @@
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="14" customWidth="1" min="1" max="1"/>
     <col width="15.08984375" customWidth="1" min="2" max="2"/>
@@ -530,7 +530,7 @@
         <v>15</v>
       </c>
       <c r="M2" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">

</xml_diff>